<commit_message>
little changes to file names for saving
</commit_message>
<xml_diff>
--- a/results/by_outcome/full_results_education_PGI_MI.xlsx
+++ b/results/by_outcome/full_results_education_PGI_MI.xlsx
@@ -483,10 +483,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H2" t="n">
-        <v>0.591627376357661</v>
+        <v>0.58841232396507</v>
       </c>
       <c r="I2" t="n">
-        <v>0.276189284272197</v>
+        <v>0.280826277319723</v>
       </c>
       <c r="J2" t="e">
         <v>#NUM!</v>
@@ -504,7 +504,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" t="n">
-        <v>0.408427527801694</v>
+        <v>0.411640923743397</v>
       </c>
     </row>
     <row r="3">
@@ -524,10 +524,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F3" t="n">
-        <v>0.605658167141403</v>
+        <v>0.603730324507612</v>
       </c>
       <c r="G3" t="n">
-        <v>0.310021511760123</v>
+        <v>0.311559776320818</v>
       </c>
       <c r="H3" t="e">
         <v>#NUM!</v>
@@ -562,13 +562,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.637296984495934</v>
+        <v>0.637358737239101</v>
       </c>
       <c r="D4" t="n">
-        <v>0.362795826096782</v>
+        <v>0.362731764845503</v>
       </c>
       <c r="E4" t="n">
-        <v>1.00009281059272</v>
+        <v>1.0000905020846</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
@@ -583,19 +583,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J4" t="n">
-        <v>0.362762157879051</v>
+        <v>0.362698939830343</v>
       </c>
       <c r="K4" t="n">
-        <v>0.309992741140584</v>
+        <v>0.311531582060349</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0140294886933653</v>
+        <v>0.0153166143440778</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0456653699226428</v>
+        <v>0.0489419839130541</v>
       </c>
       <c r="N4" t="n">
-        <v>0.324022229833949</v>
+        <v>0.326848196404427</v>
       </c>
       <c r="O4" t="e">
         <v>#NUM!</v>
@@ -640,13 +640,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.362762157879051</v>
+        <v>0.362698939830343</v>
       </c>
       <c r="D2" t="n">
-        <v>0.326483001021517</v>
+        <v>0.331220133480282</v>
       </c>
       <c r="E2" t="n">
-        <v>0.399041314736586</v>
+        <v>0.394177746180405</v>
       </c>
     </row>
     <row r="3">
@@ -657,13 +657,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.324022229833949</v>
+        <v>0.326848196404427</v>
       </c>
       <c r="D3" t="n">
-        <v>0.287534529784157</v>
+        <v>0.297364592378915</v>
       </c>
       <c r="E3" t="n">
-        <v>0.360509929883741</v>
+        <v>0.356331800429939</v>
       </c>
     </row>
     <row r="4">
@@ -674,13 +674,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>0.408427527801694</v>
+        <v>0.411640923743397</v>
       </c>
       <c r="D4" t="n">
-        <v>0.371119400563851</v>
+        <v>0.380403652512811</v>
       </c>
       <c r="E4" t="n">
-        <v>0.445735655039537</v>
+        <v>0.442878194973983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed plot axis limits
</commit_message>
<xml_diff>
--- a/results/by_outcome/full_results_education_PGI_MI.xlsx
+++ b/results/by_outcome/full_results_education_PGI_MI.xlsx
@@ -483,10 +483,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H2" t="n">
-        <v>0.58841232396507</v>
+        <v>0.589155258229011</v>
       </c>
       <c r="I2" t="n">
-        <v>0.280826277319723</v>
+        <v>0.279370328170232</v>
       </c>
       <c r="J2" t="e">
         <v>#NUM!</v>
@@ -504,7 +504,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" t="n">
-        <v>0.411640923743397</v>
+        <v>0.410898045795768</v>
       </c>
     </row>
     <row r="3">
@@ -524,10 +524,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F3" t="n">
-        <v>0.603730324507612</v>
+        <v>0.603924329216196</v>
       </c>
       <c r="G3" t="n">
-        <v>0.311559776320818</v>
+        <v>0.311741230630201</v>
       </c>
       <c r="H3" t="e">
         <v>#NUM!</v>
@@ -562,13 +562,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.637358737239101</v>
+        <v>0.63758128463405</v>
       </c>
       <c r="D4" t="n">
-        <v>0.362731764845503</v>
+        <v>0.362509198923953</v>
       </c>
       <c r="E4" t="n">
-        <v>1.0000905020846</v>
+        <v>1.000090483558</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
@@ -583,19 +583,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J4" t="n">
-        <v>0.362698939830343</v>
+        <v>0.362476400765031</v>
       </c>
       <c r="K4" t="n">
-        <v>0.311531582060349</v>
+        <v>0.31171302572226</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0153166143440778</v>
+        <v>0.0147677347384245</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0489419839130541</v>
+        <v>0.0484216450307373</v>
       </c>
       <c r="N4" t="n">
-        <v>0.326848196404427</v>
+        <v>0.326480760460685</v>
       </c>
       <c r="O4" t="e">
         <v>#NUM!</v>
@@ -640,13 +640,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.362698939830343</v>
+        <v>0.362476400765031</v>
       </c>
       <c r="D2" t="n">
-        <v>0.331220133480282</v>
+        <v>0.333980048443841</v>
       </c>
       <c r="E2" t="n">
-        <v>0.394177746180405</v>
+        <v>0.390972753086221</v>
       </c>
     </row>
     <row r="3">
@@ -657,13 +657,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.326848196404427</v>
+        <v>0.326480760460685</v>
       </c>
       <c r="D3" t="n">
-        <v>0.297364592378915</v>
+        <v>0.299440473577494</v>
       </c>
       <c r="E3" t="n">
-        <v>0.356331800429939</v>
+        <v>0.353521047343875</v>
       </c>
     </row>
     <row r="4">
@@ -674,13 +674,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>0.411640923743397</v>
+        <v>0.410898045795768</v>
       </c>
       <c r="D4" t="n">
-        <v>0.380403652512811</v>
+        <v>0.380231140088459</v>
       </c>
       <c r="E4" t="n">
-        <v>0.442878194973983</v>
+        <v>0.441564951503078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>